<commit_message>
:ok_hand: Atualização nos campos. Campo Informação do Produto removido, o campo de URL agora é preenchido na PlanilhaSku.
</commit_message>
<xml_diff>
--- a/planilhapadrão/Hercules Cobaia.xlsx
+++ b/planilhapadrão/Hercules Cobaia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\manipularPlanilhas\Planilha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Desenvolvimento\Python\Scripts Trabalho\automatizarPlanilhaVTEX\planilhapadrão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269911EF-822E-4937-9A24-631A252EB38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455993AC-E416-4314-98C0-1C8A71E2A79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A220D98B-D511-4261-A1DE-F69C6B222EA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A220D98B-D511-4261-A1DE-F69C6B222EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixa" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="348">
   <si>
     <t>_SkuEan</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>_Marca</t>
-  </si>
-  <si>
-    <t>Informações do produto</t>
   </si>
   <si>
     <t>Informações Técnicas</t>
@@ -1711,10 +1708,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6BD081A-DEC6-48D2-AA98-0A6163BE7B71}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1728,21 +1725,20 @@
     <col min="11" max="11" width="11.85546875" style="24" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="24"/>
     <col min="13" max="13" width="9.5703125" style="24" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="24"/>
-    <col min="16" max="16" width="15.85546875" style="24" customWidth="1"/>
-    <col min="17" max="18" width="9.140625" style="24"/>
-    <col min="19" max="19" width="22.7109375" style="24" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="24"/>
-    <col min="21" max="21" width="9.140625" style="24" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="24"/>
+    <col min="14" max="16" width="9.140625" style="24"/>
+    <col min="17" max="17" width="20.28515625" style="24" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" style="24" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="24"/>
+    <col min="20" max="20" width="9.140625" style="24" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>21</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>0</v>
@@ -1795,22 +1791,19 @@
       <c r="S1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="22" t="s">
-        <v>17</v>
+      <c r="T1" s="23" t="s">
+        <v>322</v>
       </c>
       <c r="U1" s="23" t="s">
-        <v>323</v>
-      </c>
-      <c r="V1" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>67393</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="5">
         <v>26</v>
@@ -1828,51 +1821,48 @@
         <v>605012134</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L2" s="24">
         <v>370</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N2" s="24">
         <v>2000179</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P2" s="24" t="s">
-        <v>83</v>
+        <v>185</v>
       </c>
       <c r="Q2" s="24" t="s">
-        <v>186</v>
+        <v>261</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>262</v>
-      </c>
-      <c r="S2" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="U2" s="24" t="s">
-        <v>324</v>
-      </c>
-      <c r="V2" s="24">
+        <v>134</v>
+      </c>
+      <c r="T2" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="U2" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>68187</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D3" s="5">
         <v>26</v>
@@ -1890,45 +1880,42 @@
         <v>605012254</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L3" s="24">
         <v>370</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N3" s="24">
         <v>2000179</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>288</v>
-      </c>
-      <c r="P3" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="S3" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>325</v>
-      </c>
-      <c r="V3" s="24">
+        <v>287</v>
+      </c>
+      <c r="R3" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="T3" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="U3" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>67385</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="5">
         <v>26</v>
@@ -1946,51 +1933,48 @@
         <v>605023002</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L4" s="24">
         <v>370</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N4" s="24">
         <v>2000179</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>83</v>
+        <v>186</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>187</v>
+        <v>262</v>
       </c>
       <c r="R4" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="S4" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="U4" s="24" t="s">
-        <v>326</v>
-      </c>
-      <c r="V4" s="24">
+        <v>122</v>
+      </c>
+      <c r="T4" s="24" t="s">
+        <v>325</v>
+      </c>
+      <c r="U4" s="24">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>67386</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="5">
         <v>26</v>
@@ -2008,51 +1992,48 @@
         <v>605023005</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L5" s="24">
         <v>370</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N5" s="24">
         <v>2000179</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P5" s="24" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>188</v>
+        <v>263</v>
       </c>
       <c r="R5" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="S5" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="U5" s="24" t="s">
-        <v>327</v>
-      </c>
-      <c r="V5" s="24">
+        <v>123</v>
+      </c>
+      <c r="T5" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="U5" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>67387</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="24">
         <v>45</v>
@@ -2073,51 +2054,48 @@
         <v>605023006</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L6" s="24">
         <v>370</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N6" s="24">
         <v>2000179</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>83</v>
+        <v>188</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>189</v>
+        <v>264</v>
       </c>
       <c r="R6" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="S6" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="U6" s="24" t="s">
-        <v>328</v>
-      </c>
-      <c r="V6" s="24">
+        <v>124</v>
+      </c>
+      <c r="T6" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="U6" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>67388</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" s="5">
         <v>26</v>
@@ -2135,51 +2113,48 @@
         <v>605023007</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L7" s="24">
         <v>370</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N7" s="24">
         <v>2000179</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>83</v>
+        <v>189</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>190</v>
+        <v>265</v>
       </c>
       <c r="R7" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="S7" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="U7" s="24" t="s">
-        <v>329</v>
-      </c>
-      <c r="V7" s="24">
+        <v>125</v>
+      </c>
+      <c r="T7" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="U7" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>67390</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="5">
         <v>26</v>
@@ -2197,51 +2172,48 @@
         <v>605037007</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L8" s="24">
         <v>370</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N8" s="24">
         <v>2000179</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>191</v>
+        <v>266</v>
       </c>
       <c r="R8" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="S8" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="U8" s="24" t="s">
-        <v>330</v>
-      </c>
-      <c r="V8" s="24">
+        <v>126</v>
+      </c>
+      <c r="T8" s="24" t="s">
+        <v>329</v>
+      </c>
+      <c r="U8" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>67391</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="5">
         <v>26</v>
@@ -2259,51 +2231,48 @@
         <v>605037008</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L9" s="24">
         <v>370</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N9" s="24">
         <v>2000179</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P9" s="24" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>192</v>
+        <v>267</v>
       </c>
       <c r="R9" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="S9" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="U9" s="24" t="s">
-        <v>331</v>
-      </c>
-      <c r="V9" s="24">
+        <v>127</v>
+      </c>
+      <c r="T9" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="U9" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>67392</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" s="5">
         <v>26</v>
@@ -2321,51 +2290,48 @@
         <v>605037009</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L10" s="24">
         <v>370</v>
       </c>
       <c r="M10" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N10" s="24">
         <v>2000179</v>
       </c>
       <c r="O10" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P10" s="24" t="s">
-        <v>83</v>
+        <v>192</v>
       </c>
       <c r="Q10" s="24" t="s">
-        <v>193</v>
+        <v>268</v>
       </c>
       <c r="R10" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="S10" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="U10" s="24" t="s">
-        <v>332</v>
-      </c>
-      <c r="V10" s="24">
+        <v>128</v>
+      </c>
+      <c r="T10" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="U10" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>67394</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D11" s="5">
         <v>26</v>
@@ -2383,51 +2349,48 @@
         <v>605038010</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L11" s="24">
         <v>370</v>
       </c>
       <c r="M11" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N11" s="24">
         <v>2000179</v>
       </c>
       <c r="O11" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>188</v>
+        <v>269</v>
       </c>
       <c r="R11" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="S11" s="24" t="s">
-        <v>206</v>
-      </c>
-      <c r="U11" s="24" t="s">
-        <v>321</v>
-      </c>
-      <c r="V11" s="24">
+        <v>205</v>
+      </c>
+      <c r="T11" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="U11" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>67395</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D12" s="5">
         <v>26</v>
@@ -2445,51 +2408,48 @@
         <v>605038011</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K12" s="24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L12" s="24">
         <v>370</v>
       </c>
       <c r="M12" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N12" s="24">
         <v>2000179</v>
       </c>
       <c r="O12" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>83</v>
+        <v>193</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>194</v>
+        <v>270</v>
       </c>
       <c r="R12" s="24" t="s">
-        <v>271</v>
-      </c>
-      <c r="S12" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="U12" s="24" t="s">
-        <v>333</v>
-      </c>
-      <c r="V12" s="24">
+        <v>129</v>
+      </c>
+      <c r="T12" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="U12" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>67396</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" s="5">
         <v>26</v>
@@ -2507,51 +2467,48 @@
         <v>605038012</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" s="24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L13" s="24">
         <v>370</v>
       </c>
       <c r="M13" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N13" s="24">
         <v>2000179</v>
       </c>
       <c r="O13" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>83</v>
+        <v>189</v>
       </c>
       <c r="Q13" s="24" t="s">
-        <v>190</v>
+        <v>271</v>
       </c>
       <c r="R13" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="S13" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="U13" s="24" t="s">
-        <v>322</v>
-      </c>
-      <c r="V13" s="24">
+        <v>204</v>
+      </c>
+      <c r="T13" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="U13" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>67398</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="5">
         <v>26</v>
@@ -2569,51 +2526,48 @@
         <v>605039010</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L14" s="24">
         <v>370</v>
       </c>
       <c r="M14" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N14" s="24">
         <v>2000179</v>
       </c>
       <c r="O14" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P14" s="24" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="Q14" s="24" t="s">
-        <v>171</v>
+        <v>272</v>
       </c>
       <c r="R14" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="S14" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="U14" s="24" t="s">
-        <v>334</v>
-      </c>
-      <c r="V14" s="24">
+        <v>130</v>
+      </c>
+      <c r="T14" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="U14" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>67399</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" s="24">
         <v>12</v>
@@ -2634,51 +2588,48 @@
         <v>605039011</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L15" s="24">
         <v>370</v>
       </c>
       <c r="M15" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N15" s="24">
         <v>2000179</v>
       </c>
       <c r="O15" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P15" s="24" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="Q15" s="24" t="s">
-        <v>172</v>
+        <v>273</v>
       </c>
       <c r="R15" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="S15" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="U15" s="24" t="s">
-        <v>335</v>
-      </c>
-      <c r="V15" s="24">
+        <v>131</v>
+      </c>
+      <c r="T15" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="U15" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>67400</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="5">
         <v>26</v>
@@ -2696,51 +2647,48 @@
         <v>605039012</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L16" s="24">
         <v>370</v>
       </c>
       <c r="M16" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N16" s="24">
         <v>2000179</v>
       </c>
       <c r="O16" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P16" s="24" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="Q16" s="24" t="s">
-        <v>173</v>
+        <v>274</v>
       </c>
       <c r="R16" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="S16" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="U16" s="24" t="s">
-        <v>336</v>
-      </c>
-      <c r="V16" s="24">
+        <v>132</v>
+      </c>
+      <c r="T16" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="U16" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>67506</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" s="5">
         <v>26</v>
@@ -2758,51 +2706,48 @@
         <v>605039013</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L17" s="24">
         <v>370</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N17" s="24">
         <v>2000179</v>
       </c>
       <c r="O17" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P17" s="24" t="s">
-        <v>85</v>
+        <v>173</v>
       </c>
       <c r="Q17" s="24" t="s">
-        <v>174</v>
+        <v>275</v>
       </c>
       <c r="R17" s="24" t="s">
-        <v>276</v>
-      </c>
-      <c r="S17" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="U17" s="24" t="s">
-        <v>337</v>
-      </c>
-      <c r="V17" s="24">
+        <v>133</v>
+      </c>
+      <c r="T17" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="U17" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>67408</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D18" s="5">
         <v>26</v>
@@ -2820,51 +2765,48 @@
         <v>605083007</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L18" s="24">
         <v>370</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N18" s="24">
         <v>2000179</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P18" s="24" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="Q18" s="24" t="s">
-        <v>175</v>
+        <v>276</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="S18" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="U18" s="24" t="s">
-        <v>338</v>
-      </c>
-      <c r="V18" s="24">
+        <v>196</v>
+      </c>
+      <c r="T18" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="U18" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>67500</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D19" s="10">
         <v>34</v>
@@ -2882,48 +2824,45 @@
         <v>605083011</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L19" s="24">
         <v>370</v>
       </c>
       <c r="M19" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N19" s="24">
         <v>2000179</v>
       </c>
       <c r="O19" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P19" s="24" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="Q19" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="R19" s="24" t="s">
-        <v>278</v>
-      </c>
-      <c r="U19" s="24" t="s">
-        <v>339</v>
-      </c>
-      <c r="V19" s="24">
+        <v>277</v>
+      </c>
+      <c r="T19" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="U19" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>67410</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D20" s="5">
         <v>34</v>
@@ -2941,51 +2880,48 @@
         <v>605083012</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L20" s="24">
         <v>370</v>
       </c>
       <c r="M20" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N20" s="24">
         <v>2000179</v>
       </c>
       <c r="O20" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P20" s="24" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="Q20" s="24" t="s">
-        <v>177</v>
+        <v>278</v>
       </c>
       <c r="R20" s="24" t="s">
-        <v>279</v>
-      </c>
-      <c r="S20" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="U20" s="24" t="s">
-        <v>340</v>
-      </c>
-      <c r="V20" s="24">
+        <v>200</v>
+      </c>
+      <c r="T20" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="U20" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>67401</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" s="5">
         <v>26</v>
@@ -3003,51 +2939,48 @@
         <v>606502009</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L21" s="24">
         <v>370</v>
       </c>
       <c r="M21" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N21" s="24">
         <v>2000179</v>
       </c>
       <c r="O21" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P21" s="24" t="s">
-        <v>87</v>
+        <v>177</v>
       </c>
       <c r="Q21" s="24" t="s">
-        <v>178</v>
+        <v>279</v>
       </c>
       <c r="R21" s="24" t="s">
-        <v>280</v>
-      </c>
-      <c r="S21" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="U21" s="24" t="s">
-        <v>341</v>
-      </c>
-      <c r="V21" s="24">
+        <v>109</v>
+      </c>
+      <c r="T21" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="U21" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>67403</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" s="10">
         <v>32</v>
@@ -3065,51 +2998,48 @@
         <v>606502414</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K22" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L22" s="24">
         <v>370</v>
       </c>
       <c r="M22" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N22" s="24">
         <v>2000179</v>
       </c>
       <c r="O22" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P22" s="24" t="s">
-        <v>87</v>
+        <v>178</v>
       </c>
       <c r="Q22" s="24" t="s">
-        <v>179</v>
+        <v>280</v>
       </c>
       <c r="R22" s="24" t="s">
-        <v>281</v>
-      </c>
-      <c r="S22" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="U22" s="24" t="s">
-        <v>342</v>
-      </c>
-      <c r="V22" s="24">
+        <v>110</v>
+      </c>
+      <c r="T22" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="U22" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>67507</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D23" s="10">
         <v>34</v>
@@ -3127,51 +3057,48 @@
         <v>606502417</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L23" s="24">
         <v>370</v>
       </c>
       <c r="M23" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N23" s="24">
         <v>2000179</v>
       </c>
       <c r="O23" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P23" s="24" t="s">
-        <v>87</v>
+        <v>179</v>
       </c>
       <c r="Q23" s="24" t="s">
-        <v>180</v>
+        <v>281</v>
       </c>
       <c r="R23" s="24" t="s">
-        <v>282</v>
-      </c>
-      <c r="S23" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="U23" s="24" t="s">
-        <v>343</v>
-      </c>
-      <c r="V23" s="24">
+        <v>111</v>
+      </c>
+      <c r="T23" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="U23" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>67498</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="5">
         <v>32</v>
@@ -3189,51 +3116,48 @@
         <v>606502419</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L24" s="24">
         <v>370</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N24" s="24">
         <v>2000179</v>
       </c>
       <c r="O24" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P24" s="24" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="Q24" s="24" t="s">
-        <v>181</v>
+        <v>282</v>
       </c>
       <c r="R24" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="S24" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="U24" s="24" t="s">
-        <v>344</v>
-      </c>
-      <c r="V24" s="24">
+        <v>112</v>
+      </c>
+      <c r="T24" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="U24" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>67404</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D25" s="5">
         <v>36</v>
@@ -3251,51 +3175,48 @@
         <v>606502421</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L25" s="24">
         <v>370</v>
       </c>
       <c r="M25" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N25" s="24">
         <v>2000179</v>
       </c>
       <c r="O25" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P25" s="24" t="s">
-        <v>87</v>
+        <v>181</v>
       </c>
       <c r="Q25" s="24" t="s">
-        <v>182</v>
+        <v>283</v>
       </c>
       <c r="R25" s="24" t="s">
-        <v>284</v>
-      </c>
-      <c r="S25" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="U25" s="24" t="s">
-        <v>345</v>
-      </c>
-      <c r="V25" s="24">
+        <v>113</v>
+      </c>
+      <c r="T25" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="U25" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>67405</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D26" s="10">
         <v>32</v>
@@ -3313,51 +3234,48 @@
         <v>606504415</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L26" s="24">
         <v>370</v>
       </c>
       <c r="M26" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N26" s="24">
         <v>2000179</v>
       </c>
       <c r="O26" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P26" s="24" t="s">
-        <v>87</v>
+        <v>182</v>
       </c>
       <c r="Q26" s="24" t="s">
-        <v>183</v>
+        <v>284</v>
       </c>
       <c r="R26" s="24" t="s">
-        <v>285</v>
-      </c>
-      <c r="S26" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="U26" s="24" t="s">
-        <v>346</v>
-      </c>
-      <c r="V26" s="24">
+        <v>114</v>
+      </c>
+      <c r="T26" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="U26" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>67406</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="10">
         <v>34</v>
@@ -3375,51 +3293,48 @@
         <v>606504418</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K27" s="24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L27" s="24">
         <v>370</v>
       </c>
       <c r="M27" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N27" s="24">
         <v>2000179</v>
       </c>
       <c r="O27" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P27" s="24" t="s">
-        <v>87</v>
+        <v>183</v>
       </c>
       <c r="Q27" s="24" t="s">
-        <v>184</v>
+        <v>285</v>
       </c>
       <c r="R27" s="24" t="s">
-        <v>286</v>
-      </c>
-      <c r="S27" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="U27" s="24" t="s">
-        <v>347</v>
-      </c>
-      <c r="V27" s="24">
+        <v>115</v>
+      </c>
+      <c r="T27" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="U27" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>67407</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D28" s="5">
         <v>34</v>
@@ -3437,42 +3352,39 @@
         <v>606504420</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L28" s="24">
         <v>370</v>
       </c>
       <c r="M28" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N28" s="24">
         <v>2000179</v>
       </c>
       <c r="O28" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P28" s="24" t="s">
-        <v>87</v>
+        <v>184</v>
       </c>
       <c r="Q28" s="24" t="s">
-        <v>185</v>
+        <v>286</v>
       </c>
       <c r="R28" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="S28" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="U28" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="V28" s="24">
+        <v>116</v>
+      </c>
+      <c r="T28" s="24" t="s">
+        <v>347</v>
+      </c>
+      <c r="U28" s="24">
         <v>1</v>
       </c>
     </row>
@@ -3510,79 +3422,79 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="5"/>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="P1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC1" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="AC1" s="20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3590,29 +3502,29 @@
         <v>67393</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="2">
         <v>605012134</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10">
@@ -3628,46 +3540,46 @@
         <v>43</v>
       </c>
       <c r="P2" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="X2" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>136</v>
-      </c>
       <c r="Y2" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Z2" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="AA2" s="5" t="s">
-        <v>208</v>
-      </c>
       <c r="AB2" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3675,29 +3587,29 @@
         <v>68187</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="2">
         <v>605012254</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9">
@@ -3713,44 +3625,44 @@
         <v>43</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R3" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="S3" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="T3" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="T3" s="13" t="s">
-        <v>160</v>
-      </c>
       <c r="U3" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V3" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W3" s="13"/>
       <c r="X3" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Y3" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3758,29 +3670,29 @@
         <v>67385</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="2">
         <v>605023002</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="27" t="s">
-        <v>26</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9">
@@ -3796,46 +3708,46 @@
         <v>43</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R4" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S4" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="T4" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="U4" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="U4" s="13" t="s">
+      <c r="V4" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W4" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="V4" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="X4" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA4" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AC4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3843,27 +3755,27 @@
         <v>67386</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="2">
         <v>605023005</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="27"/>
       <c r="I5" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9">
@@ -3879,46 +3791,46 @@
         <v>43</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R5" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S5" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="T5" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="U5" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="V5" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W5" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="V5" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W5" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="X5" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA5" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB5" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AC5" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3926,27 +3838,27 @@
         <v>67387</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="2">
         <v>605023006</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="27"/>
       <c r="I6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9">
@@ -3962,46 +3874,46 @@
         <v>43</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R6" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S6" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="T6" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T6" s="13" t="s">
+      <c r="U6" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="V6" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W6" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="V6" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W6" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="X6" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AB6" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AC6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4009,27 +3921,27 @@
         <v>67388</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="2">
         <v>605023007</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9">
@@ -4045,46 +3957,46 @@
         <v>43</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R7" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S7" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="T7" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="U7" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="V7" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W7" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="V7" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W7" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="X7" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AB7" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AC7" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4092,27 +4004,27 @@
         <v>67390</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="2">
         <v>605037007</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="27"/>
       <c r="I8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9">
@@ -4128,46 +4040,46 @@
         <v>43</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R8" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S8" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="T8" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T8" s="13" t="s">
+      <c r="U8" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="U8" s="13" t="s">
+      <c r="V8" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W8" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="V8" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W8" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="X8" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AC8" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4175,27 +4087,27 @@
         <v>67391</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="2">
         <v>605037008</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9">
@@ -4211,46 +4123,46 @@
         <v>43</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R9" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S9" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="S9" s="13" t="s">
+      <c r="T9" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T9" s="13" t="s">
+      <c r="U9" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="U9" s="13" t="s">
+      <c r="V9" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W9" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="V9" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W9" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="X9" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Z9" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA9" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB9" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AC9" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4258,27 +4170,27 @@
         <v>67392</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="2">
         <v>605037009</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="27"/>
       <c r="I10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9">
@@ -4294,46 +4206,46 @@
         <v>43</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R10" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S10" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="S10" s="13" t="s">
+      <c r="T10" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="U10" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="U10" s="13" t="s">
+      <c r="V10" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W10" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="V10" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W10" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="X10" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Z10" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AB10" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AC10" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4341,30 +4253,30 @@
         <v>67394</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="2">
         <v>605038010</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="27"/>
       <c r="I11" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L11" s="9">
         <v>15</v>
@@ -4379,46 +4291,46 @@
         <v>43</v>
       </c>
       <c r="P11" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="U11" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="V11" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W11" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="X11" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="Z11" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="Q11" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="R11" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="S11" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="T11" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="U11" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="V11" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W11" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="X11" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y11" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="Z11" s="5" t="s">
-        <v>207</v>
-      </c>
       <c r="AA11" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AB11" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AC11" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4426,27 +4338,27 @@
         <v>67395</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="2">
         <v>605038011</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9">
@@ -4462,46 +4374,46 @@
         <v>43</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R12" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S12" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="S12" s="13" t="s">
+      <c r="T12" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T12" s="13" t="s">
+      <c r="U12" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="U12" s="13" t="s">
+      <c r="V12" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W12" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="V12" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W12" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="X12" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Y12" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Z12" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA12" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AB12" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AC12" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4509,30 +4421,30 @@
         <v>67396</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="2">
         <v>605038012</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L13" s="9">
         <v>19</v>
@@ -4547,46 +4459,46 @@
         <v>43</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R13" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S13" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="S13" s="13" t="s">
+      <c r="T13" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T13" s="13" t="s">
+      <c r="U13" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="U13" s="13" t="s">
+      <c r="V13" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="W13" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="V13" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="W13" s="13" t="s">
-        <v>157</v>
-      </c>
       <c r="X13" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Y13" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Z13" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AB13" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AC13" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4594,29 +4506,29 @@
         <v>67398</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="2">
         <v>605039010</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="28" t="s">
-        <v>30</v>
-      </c>
       <c r="I14" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9">
@@ -4632,44 +4544,44 @@
         <v>43</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R14" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="S14" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="S14" s="13" t="s">
+      <c r="T14" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="T14" s="13" t="s">
+      <c r="U14" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="V14" s="13" t="s">
         <v>163</v>
-      </c>
-      <c r="U14" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="V14" s="13" t="s">
-        <v>164</v>
       </c>
       <c r="W14" s="13"/>
       <c r="X14" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Y14" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA14" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AB14" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AC14" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4677,27 +4589,27 @@
         <v>67399</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="2">
         <v>605039011</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9">
@@ -4713,44 +4625,44 @@
         <v>43</v>
       </c>
       <c r="P15" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R15" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="S15" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="S15" s="13" t="s">
+      <c r="T15" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="T15" s="13" t="s">
+      <c r="U15" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="V15" s="13" t="s">
         <v>163</v>
-      </c>
-      <c r="U15" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="V15" s="13" t="s">
-        <v>164</v>
       </c>
       <c r="W15" s="13"/>
       <c r="X15" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Z15" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AB15" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AC15" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4758,27 +4670,27 @@
         <v>67400</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="2">
         <v>605039012</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" s="29"/>
       <c r="I16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9">
@@ -4794,44 +4706,44 @@
         <v>43</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R16" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="S16" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="S16" s="13" t="s">
+      <c r="T16" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="T16" s="13" t="s">
+      <c r="U16" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="V16" s="13" t="s">
         <v>163</v>
-      </c>
-      <c r="U16" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="V16" s="13" t="s">
-        <v>164</v>
       </c>
       <c r="W16" s="13"/>
       <c r="X16" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Y16" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Z16" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA16" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AB16" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AC16" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4839,27 +4751,27 @@
         <v>67506</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="2">
         <v>605039013</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H17" s="29"/>
       <c r="I17" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9">
@@ -4875,44 +4787,44 @@
         <v>43</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R17" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="S17" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="S17" s="13" t="s">
+      <c r="T17" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="T17" s="13" t="s">
+      <c r="U17" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="V17" s="13" t="s">
         <v>163</v>
-      </c>
-      <c r="U17" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="V17" s="13" t="s">
-        <v>164</v>
       </c>
       <c r="W17" s="13"/>
       <c r="X17" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Y17" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Z17" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA17" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AB17" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AC17" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4920,29 +4832,29 @@
         <v>67408</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="2">
         <v>605083007</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H18" s="30" t="s">
-        <v>32</v>
-      </c>
       <c r="I18" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9">
@@ -4958,42 +4870,42 @@
         <v>43</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R18" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="S18" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="S18" s="13" t="s">
-        <v>166</v>
-      </c>
       <c r="T18" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U18" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V18" s="13"/>
       <c r="W18" s="13"/>
       <c r="X18" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Y18" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Z18" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AB18" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AC18" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5001,27 +4913,27 @@
         <v>67500</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="2">
         <v>605083011</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H19" s="31"/>
       <c r="I19" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9">
@@ -5037,42 +4949,42 @@
         <v>40</v>
       </c>
       <c r="P19" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R19" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="S19" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="S19" s="13" t="s">
-        <v>166</v>
-      </c>
       <c r="T19" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U19" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V19" s="13"/>
       <c r="W19" s="13"/>
       <c r="X19" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y19" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Z19" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA19" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AB19" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AC19" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5080,27 +4992,27 @@
         <v>67410</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="2">
         <v>605083012</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H20" s="31"/>
       <c r="I20" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9">
@@ -5116,42 +5028,42 @@
         <v>50</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R20" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="S20" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="S20" s="13" t="s">
-        <v>166</v>
-      </c>
       <c r="T20" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="U20" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="V20" s="13"/>
       <c r="W20" s="13"/>
       <c r="X20" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Z20" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA20" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AB20" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AC20" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5159,29 +5071,29 @@
         <v>67401</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="2">
         <v>606502009</v>
       </c>
       <c r="G21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="32" t="s">
-        <v>34</v>
-      </c>
       <c r="I21" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L21" s="5">
         <v>18</v>
@@ -5196,42 +5108,42 @@
         <v>43</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R21" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="S21" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="T21" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="S21" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="T21" s="13" t="s">
-        <v>167</v>
-      </c>
       <c r="U21" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V21" s="13"/>
       <c r="W21" s="13"/>
       <c r="X21" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Z21" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA21" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AB21" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AC21" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5239,27 +5151,27 @@
         <v>67403</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="2">
         <v>606502414</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H22" s="33"/>
       <c r="I22" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L22" s="5">
         <v>28</v>
@@ -5274,42 +5186,42 @@
         <v>36</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R22" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="S22" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="T22" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="S22" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="T22" s="13" t="s">
-        <v>167</v>
-      </c>
       <c r="U22" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V22" s="13"/>
       <c r="W22" s="13"/>
       <c r="X22" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Y22" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Z22" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA22" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AB22" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AC22" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5317,27 +5229,27 @@
         <v>67507</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="2">
         <v>606502417</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H23" s="33"/>
       <c r="I23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L23" s="9">
         <v>64</v>
@@ -5352,42 +5264,42 @@
         <v>40</v>
       </c>
       <c r="P23" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R23" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="S23" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="T23" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="S23" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="T23" s="13" t="s">
-        <v>167</v>
-      </c>
       <c r="U23" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V23" s="13"/>
       <c r="W23" s="13"/>
       <c r="X23" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y23" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z23" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA23" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AB23" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AC23" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5395,27 +5307,27 @@
         <v>67498</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="2">
         <v>606502419</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H24" s="33"/>
       <c r="I24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L24" s="5">
         <v>75</v>
@@ -5430,42 +5342,42 @@
         <v>50</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R24" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="S24" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="T24" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="S24" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="T24" s="13" t="s">
-        <v>167</v>
-      </c>
       <c r="U24" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V24" s="13"/>
       <c r="W24" s="13"/>
       <c r="X24" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Y24" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Z24" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA24" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AB24" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AC24" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5473,27 +5385,27 @@
         <v>67404</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="2">
         <v>606502421</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H25" s="33"/>
       <c r="I25" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L25" s="5">
         <v>90</v>
@@ -5508,42 +5420,42 @@
         <v>50</v>
       </c>
       <c r="P25" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R25" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="S25" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="T25" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="S25" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="T25" s="13" t="s">
-        <v>167</v>
-      </c>
       <c r="U25" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V25" s="13"/>
       <c r="W25" s="13"/>
       <c r="X25" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Y25" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Z25" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA25" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AB25" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AC25" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5551,27 +5463,27 @@
         <v>67405</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="2">
         <v>606504415</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H26" s="33"/>
       <c r="I26" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L26" s="5">
         <v>35</v>
@@ -5586,42 +5498,42 @@
         <v>36</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R26" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="S26" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="T26" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="S26" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="T26" s="13" t="s">
-        <v>167</v>
-      </c>
       <c r="U26" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V26" s="13"/>
       <c r="W26" s="13"/>
       <c r="X26" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Y26" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z26" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA26" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AB26" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AC26" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5629,27 +5541,27 @@
         <v>67406</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="2">
         <v>606504418</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H27" s="33"/>
       <c r="I27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L27" s="5">
         <v>64</v>
@@ -5664,42 +5576,42 @@
         <v>40</v>
       </c>
       <c r="P27" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R27" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="S27" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="T27" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="S27" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="T27" s="13" t="s">
-        <v>167</v>
-      </c>
       <c r="U27" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V27" s="13"/>
       <c r="W27" s="13"/>
       <c r="X27" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Y27" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z27" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA27" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AB27" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AC27" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5707,27 +5619,27 @@
         <v>67407</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="2">
         <v>606504420</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H28" s="33"/>
       <c r="I28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L28" s="5">
         <v>75</v>
@@ -5742,42 +5654,42 @@
         <v>50</v>
       </c>
       <c r="P28" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R28" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="S28" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="T28" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="S28" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="T28" s="13" t="s">
-        <v>167</v>
-      </c>
       <c r="U28" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V28" s="13"/>
       <c r="W28" s="13"/>
       <c r="X28" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Y28" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Z28" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA28" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AB28" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AC28" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
stable version new feat checking ID's, complete
</commit_message>
<xml_diff>
--- a/planilhapadrão/Hercules Cobaia.xlsx
+++ b/planilhapadrão/Hercules Cobaia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\Python\automatizarPlanilhaVTEX\planilhapadrão\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Python\automatizar_planilha_vtex\planilhapadrão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31BB3F0-3B5D-430E-9C98-35B025E0FB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3494C9C-828B-4823-B764-44880B80D6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A220D98B-D511-4261-A1DE-F69C6B222EA8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A220D98B-D511-4261-A1DE-F69C6B222EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixa" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="276">
   <si>
     <t>_SkuEan</t>
   </si>
@@ -882,84 +882,6 @@
     <t>O Motor Monofásico Hércules IP 21 4P 3 CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
   </si>
   <si>
-    <t>O Motor Bifásico Hércules  4P 2CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 2P 1/2CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 2P 1CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 2P 1.1/2CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 2P 2CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 4P 1CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 4P 1.1/2  alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 4P 2CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 B3D 2P 1CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 2P 1,5CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 21 B3D 2P 2CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 21 / IR3 ECO 4P 1CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 21 / IR3 ECO 4P 1,5CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 21 / IR3 ECO 4P 2CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 21 / IR3 ECO 4P 3CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 55 2P 2CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 55 2P 7,5CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Monofásico Hércules IP 55 2P 10CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 55 IR3 2P 2CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 55 IR3 2P 5CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 55 IR3 2P 7,5CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 55 IR3 2P 10CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 55 IR3 2P 15CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 55 IR3 4P 5CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 55 IR3 4P 7,5CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
-    <t>O Motor Trifásico Hércules IP 55 IR3 4P 10CV alia a mais alta tecnologia e rendimento a um preço acessível! Compre barato na Ferimport!</t>
-  </si>
-  <si>
     <t>motor-monofasico-hercules-ip-21-b3d-2p-1cv</t>
   </si>
   <si>
@@ -972,403 +894,19 @@
     <t>motor-monofasico-hercules-ip-21-4p-3-cv</t>
   </si>
   <si>
-    <t>motor-bifasico-hercules-4p-2cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-21-2p-1-2cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-21-2p-1cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-21-2p-1-1-2cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-21-2p-2cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-21-4p-1cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-21-4p-1-1-2</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-21-4p-2cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-21-2p-15cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-21-ir3-eco-4p-1cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-21-ir3-eco-4p-15cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-21-ir3-eco-4p-2cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-21-ir3-eco-4p-3cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-55-2p-2cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-55-2p-75cv</t>
-  </si>
-  <si>
-    <t>motor-monofasico-hercules-ip-55-2p-10cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-55-ir3-2p-2cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-55-ir3-2p-5cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-55-ir3-2p-75cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-55-ir3-2p-10cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-55-ir3-2p-15cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-55-ir3-4p-5cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-55-ir3-4p-75cv</t>
-  </si>
-  <si>
-    <t>motor-trifasico-hercules-ip-55-ir3-4p-10cv</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
     <t>70000TEC</t>
   </si>
   <si>
-    <t>70001TEC</t>
-  </si>
-  <si>
-    <t>70002TEC</t>
-  </si>
-  <si>
-    <t>70003TEC</t>
-  </si>
-  <si>
-    <t>70004TEC</t>
-  </si>
-  <si>
-    <t>70005TEC</t>
-  </si>
-  <si>
-    <t>70006TEC</t>
-  </si>
-  <si>
-    <t>70007TEC</t>
-  </si>
-  <si>
-    <t>70008TEC</t>
-  </si>
-  <si>
-    <t>70009TEC</t>
-  </si>
-  <si>
-    <t>70010TEC</t>
-  </si>
-  <si>
-    <t>70011TEC</t>
-  </si>
-  <si>
-    <t>70012TEC</t>
-  </si>
-  <si>
-    <t>70013TEC</t>
-  </si>
-  <si>
-    <t>70014TEC</t>
-  </si>
-  <si>
-    <t>70015TEC</t>
-  </si>
-  <si>
-    <t>70016TEC</t>
-  </si>
-  <si>
-    <t>70017TEC</t>
-  </si>
-  <si>
-    <t>70018TEC</t>
-  </si>
-  <si>
-    <t>70019TEC</t>
-  </si>
-  <si>
-    <t>70020TEC</t>
-  </si>
-  <si>
-    <t>70021TEC</t>
-  </si>
-  <si>
-    <t>70022TEC</t>
-  </si>
-  <si>
-    <t>70023TEC</t>
-  </si>
-  <si>
-    <t>70024TEC</t>
-  </si>
-  <si>
-    <t>70025TEC</t>
-  </si>
-  <si>
-    <t>70026TEC</t>
-  </si>
-  <si>
     <t>70000FOR</t>
   </si>
   <si>
-    <t>70001FOR</t>
-  </si>
-  <si>
-    <t>70002FOR</t>
-  </si>
-  <si>
-    <t>70003FOR</t>
-  </si>
-  <si>
-    <t>70004FOR</t>
-  </si>
-  <si>
-    <t>70005FOR</t>
-  </si>
-  <si>
-    <t>70006FOR</t>
-  </si>
-  <si>
-    <t>70007FOR</t>
-  </si>
-  <si>
-    <t>70008FOR</t>
-  </si>
-  <si>
-    <t>70009FOR</t>
-  </si>
-  <si>
-    <t>70010FOR</t>
-  </si>
-  <si>
-    <t>70011FOR</t>
-  </si>
-  <si>
-    <t>70012FOR</t>
-  </si>
-  <si>
-    <t>70013FOR</t>
-  </si>
-  <si>
-    <t>70014FOR</t>
-  </si>
-  <si>
-    <t>70015FOR</t>
-  </si>
-  <si>
-    <t>70016FOR</t>
-  </si>
-  <si>
-    <t>70017FOR</t>
-  </si>
-  <si>
-    <t>70018FOR</t>
-  </si>
-  <si>
-    <t>70019FOR</t>
-  </si>
-  <si>
-    <t>70020FOR</t>
-  </si>
-  <si>
-    <t>70021FOR</t>
-  </si>
-  <si>
-    <t>70022FOR</t>
-  </si>
-  <si>
-    <t>70023FOR</t>
-  </si>
-  <si>
-    <t>70024FOR</t>
-  </si>
-  <si>
-    <t>70025FOR</t>
-  </si>
-  <si>
-    <t>70026FOR</t>
-  </si>
-  <si>
     <t>70000DESC</t>
   </si>
   <si>
-    <t>70001DESC</t>
-  </si>
-  <si>
-    <t>70002DESC</t>
-  </si>
-  <si>
-    <t>70003DESC</t>
-  </si>
-  <si>
-    <t>70004DESC</t>
-  </si>
-  <si>
-    <t>70005DESC</t>
-  </si>
-  <si>
-    <t>70006DESC</t>
-  </si>
-  <si>
-    <t>70007DESC</t>
-  </si>
-  <si>
-    <t>70008DESC</t>
-  </si>
-  <si>
-    <t>70009DESC</t>
-  </si>
-  <si>
-    <t>70010DESC</t>
-  </si>
-  <si>
-    <t>70011DESC</t>
-  </si>
-  <si>
-    <t>70012DESC</t>
-  </si>
-  <si>
-    <t>70013DESC</t>
-  </si>
-  <si>
-    <t>70014DESC</t>
-  </si>
-  <si>
-    <t>70015DESC</t>
-  </si>
-  <si>
-    <t>70016DESC</t>
-  </si>
-  <si>
-    <t>70017DESC</t>
-  </si>
-  <si>
-    <t>70018DESC</t>
-  </si>
-  <si>
-    <t>70019DESC</t>
-  </si>
-  <si>
-    <t>70020DESC</t>
-  </si>
-  <si>
-    <t>70021DESC</t>
-  </si>
-  <si>
-    <t>70022DESC</t>
-  </si>
-  <si>
-    <t>70023DESC</t>
-  </si>
-  <si>
-    <t>70024DESC</t>
-  </si>
-  <si>
-    <t>70025DESC</t>
-  </si>
-  <si>
-    <t>70026DESC</t>
-  </si>
-  <si>
     <t>70000Hércules</t>
-  </si>
-  <si>
-    <t>70001Hércules</t>
-  </si>
-  <si>
-    <t>70002Hércules</t>
-  </si>
-  <si>
-    <t>70003Hércules</t>
-  </si>
-  <si>
-    <t>70004Hércules</t>
-  </si>
-  <si>
-    <t>70005Hércules</t>
-  </si>
-  <si>
-    <t>70006Hércules</t>
-  </si>
-  <si>
-    <t>70007Hércules</t>
-  </si>
-  <si>
-    <t>70008Hércules</t>
-  </si>
-  <si>
-    <t>70009Hércules</t>
-  </si>
-  <si>
-    <t>70010Hércules</t>
-  </si>
-  <si>
-    <t>70011Hércules</t>
-  </si>
-  <si>
-    <t>70012Hércules</t>
-  </si>
-  <si>
-    <t>70013Hércules</t>
-  </si>
-  <si>
-    <t>70014Hércules</t>
-  </si>
-  <si>
-    <t>70015Hércules</t>
-  </si>
-  <si>
-    <t>70016Hércules</t>
-  </si>
-  <si>
-    <t>70017Hércules</t>
-  </si>
-  <si>
-    <t>70018Hércules</t>
-  </si>
-  <si>
-    <t>70019Hércules</t>
-  </si>
-  <si>
-    <t>70020Hércules</t>
-  </si>
-  <si>
-    <t>70021Hércules</t>
-  </si>
-  <si>
-    <t>70022Hércules</t>
-  </si>
-  <si>
-    <t>70023Hércules</t>
-  </si>
-  <si>
-    <t>70024Hércules</t>
-  </si>
-  <si>
-    <t>70025Hércules</t>
-  </si>
-  <si>
-    <t>70026Hércules</t>
   </si>
   <si>
     <t>Vídeo do produto</t>
@@ -1381,7 +919,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1428,8 +966,14 @@
       <color theme="1"/>
       <name val="Roboto Condensed"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F40"/>
+      <name val="Ubuntu"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1514,6 +1058,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1528,7 +1078,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1600,12 +1150,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1954,10 +1514,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6BD081A-DEC6-48D2-AA98-0A6163BE7B71}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1983,7 +1543,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>320</v>
+        <v>270</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>19</v>
@@ -2037,1720 +1597,87 @@
         <v>15</v>
       </c>
       <c r="T1" s="22" t="s">
-        <v>429</v>
+        <v>275</v>
       </c>
       <c r="U1" s="23" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="V1" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="26">
         <v>67393</v>
       </c>
-      <c r="B2" s="2">
-        <v>70000</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="30">
+        <v>72450</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="5">
+      <c r="D2" s="27"/>
+      <c r="E2" s="28">
         <v>26</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="28">
         <v>24</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="28">
         <v>43</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="29">
         <v>22000</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="27">
         <v>605012134</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="27">
         <v>370</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="27" t="s">
         <v>260</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="27">
         <v>2000179</v>
       </c>
-      <c r="P2" s="24" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="V2" s="24">
+      <c r="P2" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="T2" s="26"/>
+      <c r="U2" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="V2" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>68187</v>
-      </c>
-      <c r="B3" s="2">
-        <v>70001</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="5">
-        <v>26</v>
-      </c>
-      <c r="F3" s="5">
-        <v>24</v>
-      </c>
-      <c r="G3" s="5">
-        <v>43</v>
-      </c>
-      <c r="H3" s="25">
-        <v>19000</v>
-      </c>
-      <c r="I3" s="24">
-        <v>605012254</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="M3" s="24">
-        <v>370</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O3" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P3" s="24" t="s">
-        <v>403</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="T3" s="2"/>
-      <c r="U3" s="24" t="s">
-        <v>296</v>
-      </c>
-      <c r="V3" s="24">
-        <v>1</v>
+      <c r="B3" s="30">
+        <v>72447</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>67385</v>
-      </c>
-      <c r="B4" s="2">
-        <v>70002</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="5">
-        <v>26</v>
-      </c>
-      <c r="F4" s="5">
-        <v>24</v>
-      </c>
-      <c r="G4" s="5">
-        <v>43</v>
-      </c>
-      <c r="H4" s="25">
-        <v>10000</v>
-      </c>
-      <c r="I4" s="24">
-        <v>605023002</v>
-      </c>
-      <c r="J4" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L4" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="M4" s="24">
-        <v>370</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O4" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P4" s="24" t="s">
-        <v>404</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="T4" s="2"/>
-      <c r="U4" s="24" t="s">
-        <v>297</v>
-      </c>
-      <c r="V4" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>67386</v>
-      </c>
-      <c r="B5" s="2">
-        <v>70003</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="5">
-        <v>26</v>
-      </c>
-      <c r="F5" s="5">
-        <v>24</v>
-      </c>
-      <c r="G5" s="5">
-        <v>43</v>
-      </c>
-      <c r="H5" s="25">
-        <v>15000</v>
-      </c>
-      <c r="I5" s="24">
-        <v>605023005</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="M5" s="24">
-        <v>370</v>
-      </c>
-      <c r="N5" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O5" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P5" s="24" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="T5" s="2"/>
-      <c r="U5" s="24" t="s">
-        <v>298</v>
-      </c>
-      <c r="V5" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>67387</v>
-      </c>
-      <c r="B6" s="2">
-        <v>70004</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="24">
-        <v>45</v>
-      </c>
-      <c r="E6" s="5">
-        <v>26</v>
-      </c>
-      <c r="F6" s="5">
-        <v>24</v>
-      </c>
-      <c r="G6" s="5">
-        <v>43</v>
-      </c>
-      <c r="H6" s="25">
-        <v>10000</v>
-      </c>
-      <c r="I6" s="24">
-        <v>605023006</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L6" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="M6" s="24">
-        <v>370</v>
-      </c>
-      <c r="N6" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O6" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="T6" s="2"/>
-      <c r="U6" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="V6" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>67388</v>
-      </c>
-      <c r="B7" s="2">
-        <v>70005</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="5">
-        <v>26</v>
-      </c>
-      <c r="F7" s="5">
-        <v>24</v>
-      </c>
-      <c r="G7" s="5">
-        <v>43</v>
-      </c>
-      <c r="H7" s="25">
-        <v>19000</v>
-      </c>
-      <c r="I7" s="24">
-        <v>605023007</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="K7" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="M7" s="24">
-        <v>370</v>
-      </c>
-      <c r="N7" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O7" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P7" s="24" t="s">
-        <v>407</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="V7" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>67390</v>
-      </c>
-      <c r="B8" s="2">
-        <v>70006</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="5">
-        <v>26</v>
-      </c>
-      <c r="F8" s="5">
-        <v>24</v>
-      </c>
-      <c r="G8" s="5">
-        <v>43</v>
-      </c>
-      <c r="H8" s="25">
-        <v>15000</v>
-      </c>
-      <c r="I8" s="24">
-        <v>605037007</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>271</v>
-      </c>
-      <c r="M8" s="24">
-        <v>370</v>
-      </c>
-      <c r="N8" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O8" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P8" s="24" t="s">
-        <v>408</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="T8" s="2"/>
-      <c r="U8" s="24" t="s">
-        <v>301</v>
-      </c>
-      <c r="V8" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>67391</v>
-      </c>
-      <c r="B9" s="2">
-        <v>70007</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="5">
-        <v>26</v>
-      </c>
-      <c r="F9" s="5">
-        <v>24</v>
-      </c>
-      <c r="G9" s="5">
-        <v>43</v>
-      </c>
-      <c r="H9" s="25">
-        <v>16000</v>
-      </c>
-      <c r="I9" s="24">
-        <v>605037008</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="M9" s="24">
-        <v>370</v>
-      </c>
-      <c r="N9" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O9" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P9" s="24" t="s">
-        <v>409</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="T9" s="2"/>
-      <c r="U9" s="24" t="s">
-        <v>302</v>
-      </c>
-      <c r="V9" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>67392</v>
-      </c>
-      <c r="B10" s="2">
-        <v>70008</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" s="5">
-        <v>26</v>
-      </c>
-      <c r="F10" s="5">
-        <v>24</v>
-      </c>
-      <c r="G10" s="5">
-        <v>43</v>
-      </c>
-      <c r="H10" s="25">
-        <v>20000</v>
-      </c>
-      <c r="I10" s="24">
-        <v>605037009</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L10" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="M10" s="24">
-        <v>370</v>
-      </c>
-      <c r="N10" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O10" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P10" s="24" t="s">
-        <v>410</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="T10" s="2"/>
-      <c r="U10" s="24" t="s">
-        <v>303</v>
-      </c>
-      <c r="V10" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>67394</v>
-      </c>
-      <c r="B11" s="2">
-        <v>70009</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="E11" s="5">
-        <v>26</v>
-      </c>
-      <c r="F11" s="5">
-        <v>24</v>
-      </c>
-      <c r="G11" s="5">
-        <v>43</v>
-      </c>
-      <c r="H11" s="25">
-        <v>15000</v>
-      </c>
-      <c r="I11" s="24">
-        <v>605038010</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="K11" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L11" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="M11" s="24">
-        <v>370</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O11" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P11" s="24" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="T11" s="2"/>
-      <c r="U11" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="V11" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>67395</v>
-      </c>
-      <c r="B12" s="2">
-        <v>70010</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="5">
-        <v>26</v>
-      </c>
-      <c r="F12" s="5">
-        <v>24</v>
-      </c>
-      <c r="G12" s="5">
-        <v>43</v>
-      </c>
-      <c r="H12" s="25">
-        <v>18000</v>
-      </c>
-      <c r="I12" s="24">
-        <v>605038011</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="K12" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="M12" s="24">
-        <v>370</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O12" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P12" s="24" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="T12" s="2"/>
-      <c r="U12" s="24" t="s">
-        <v>304</v>
-      </c>
-      <c r="V12" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>67396</v>
-      </c>
-      <c r="B13" s="2">
-        <v>70011</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="E13" s="5">
-        <v>26</v>
-      </c>
-      <c r="F13" s="5">
-        <v>24</v>
-      </c>
-      <c r="G13" s="5">
-        <v>43</v>
-      </c>
-      <c r="H13" s="25">
-        <v>19000</v>
-      </c>
-      <c r="I13" s="24">
-        <v>605038012</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="K13" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>276</v>
-      </c>
-      <c r="M13" s="24">
-        <v>370</v>
-      </c>
-      <c r="N13" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O13" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>413</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="T13" s="2"/>
-      <c r="U13" s="24" t="s">
-        <v>293</v>
-      </c>
-      <c r="V13" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>67398</v>
-      </c>
-      <c r="B14" s="2">
-        <v>70012</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="5">
-        <v>26</v>
-      </c>
-      <c r="F14" s="5">
-        <v>24</v>
-      </c>
-      <c r="G14" s="5">
-        <v>43</v>
-      </c>
-      <c r="H14" s="25">
-        <v>15000</v>
-      </c>
-      <c r="I14" s="24">
-        <v>605039010</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="K14" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="L14" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="M14" s="24">
-        <v>370</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O14" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P14" s="24" t="s">
-        <v>414</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="T14" s="2"/>
-      <c r="U14" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="V14" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>67399</v>
-      </c>
-      <c r="B15" s="2">
-        <v>70013</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="24">
-        <v>12</v>
-      </c>
-      <c r="E15" s="5">
-        <v>26</v>
-      </c>
-      <c r="F15" s="5">
-        <v>24</v>
-      </c>
-      <c r="G15" s="5">
-        <v>43</v>
-      </c>
-      <c r="H15" s="25">
-        <v>18000</v>
-      </c>
-      <c r="I15" s="24">
-        <v>605039011</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="K15" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>278</v>
-      </c>
-      <c r="M15" s="24">
-        <v>370</v>
-      </c>
-      <c r="N15" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O15" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P15" s="24" t="s">
-        <v>415</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="T15" s="2"/>
-      <c r="U15" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="V15" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>67400</v>
-      </c>
-      <c r="B16" s="2">
-        <v>70014</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="5">
-        <v>26</v>
-      </c>
-      <c r="F16" s="5">
-        <v>24</v>
-      </c>
-      <c r="G16" s="5">
-        <v>43</v>
-      </c>
-      <c r="H16" s="25">
-        <v>20000</v>
-      </c>
-      <c r="I16" s="24">
-        <v>605039012</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="K16" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>279</v>
-      </c>
-      <c r="M16" s="24">
-        <v>370</v>
-      </c>
-      <c r="N16" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O16" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P16" s="24" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="T16" s="2"/>
-      <c r="U16" s="24" t="s">
-        <v>307</v>
-      </c>
-      <c r="V16" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>67506</v>
-      </c>
-      <c r="B17" s="2">
-        <v>70015</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="5">
-        <v>26</v>
-      </c>
-      <c r="F17" s="5">
-        <v>24</v>
-      </c>
-      <c r="G17" s="5">
-        <v>43</v>
-      </c>
-      <c r="H17" s="25">
-        <v>22000</v>
-      </c>
-      <c r="I17" s="24">
-        <v>605039013</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="K17" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="L17" s="24" t="s">
-        <v>280</v>
-      </c>
-      <c r="M17" s="24">
-        <v>370</v>
-      </c>
-      <c r="N17" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O17" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P17" s="24" t="s">
-        <v>417</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="T17" s="2"/>
-      <c r="U17" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="V17" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>67408</v>
-      </c>
-      <c r="B18" s="2">
-        <v>70016</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="E18" s="5">
-        <v>26</v>
-      </c>
-      <c r="F18" s="5">
-        <v>24</v>
-      </c>
-      <c r="G18" s="5">
-        <v>43</v>
-      </c>
-      <c r="H18" s="25">
-        <v>20000</v>
-      </c>
-      <c r="I18" s="24">
-        <v>605083007</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="K18" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="L18" s="24" t="s">
-        <v>281</v>
-      </c>
-      <c r="M18" s="24">
-        <v>370</v>
-      </c>
-      <c r="N18" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O18" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P18" s="24" t="s">
-        <v>418</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="T18" s="2"/>
-      <c r="U18" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="V18" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>67500</v>
-      </c>
-      <c r="B19" s="2">
-        <v>70017</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="E19" s="10">
-        <v>34</v>
-      </c>
-      <c r="F19" s="10">
-        <v>24</v>
-      </c>
-      <c r="G19" s="10">
-        <v>40</v>
-      </c>
-      <c r="H19" s="25">
-        <v>64000</v>
-      </c>
-      <c r="I19" s="24">
-        <v>605083011</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="K19" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="L19" s="24" t="s">
-        <v>282</v>
-      </c>
-      <c r="M19" s="24">
-        <v>370</v>
-      </c>
-      <c r="N19" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O19" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P19" s="24" t="s">
-        <v>419</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="T19" s="2"/>
-      <c r="U19" s="24" t="s">
-        <v>310</v>
-      </c>
-      <c r="V19" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>67410</v>
-      </c>
-      <c r="B20" s="2">
-        <v>70018</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="E20" s="5">
-        <v>34</v>
-      </c>
-      <c r="F20" s="5">
-        <v>38</v>
-      </c>
-      <c r="G20" s="5">
-        <v>50</v>
-      </c>
-      <c r="H20" s="25">
-        <v>75000</v>
-      </c>
-      <c r="I20" s="24">
-        <v>605083012</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="M20" s="24">
-        <v>370</v>
-      </c>
-      <c r="N20" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O20" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P20" s="24" t="s">
-        <v>420</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="S20" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="T20" s="2"/>
-      <c r="U20" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="V20" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>67401</v>
-      </c>
-      <c r="B21" s="2">
-        <v>70019</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="5">
-        <v>26</v>
-      </c>
-      <c r="F21" s="5">
-        <v>24</v>
-      </c>
-      <c r="G21" s="5">
-        <v>43</v>
-      </c>
-      <c r="H21" s="25">
-        <v>18000</v>
-      </c>
-      <c r="I21" s="24">
-        <v>606502009</v>
-      </c>
-      <c r="J21" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="K21" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L21" s="24" t="s">
-        <v>284</v>
-      </c>
-      <c r="M21" s="24">
-        <v>370</v>
-      </c>
-      <c r="N21" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O21" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P21" s="24" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="T21" s="2"/>
-      <c r="U21" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="V21" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>67403</v>
-      </c>
-      <c r="B22" s="2">
-        <v>70020</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="10">
-        <v>32</v>
-      </c>
-      <c r="F22" s="10">
-        <v>22</v>
-      </c>
-      <c r="G22" s="10">
-        <v>36</v>
-      </c>
-      <c r="H22" s="25">
-        <v>28000</v>
-      </c>
-      <c r="I22" s="24">
-        <v>606502414</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K22" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L22" s="24" t="s">
-        <v>285</v>
-      </c>
-      <c r="M22" s="24">
-        <v>370</v>
-      </c>
-      <c r="N22" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O22" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P22" s="24" t="s">
-        <v>422</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="T22" s="2"/>
-      <c r="U22" s="24" t="s">
-        <v>313</v>
-      </c>
-      <c r="V22" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>67507</v>
-      </c>
-      <c r="B23" s="2">
-        <v>70021</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E23" s="10">
-        <v>34</v>
-      </c>
-      <c r="F23" s="10">
-        <v>24</v>
-      </c>
-      <c r="G23" s="10">
-        <v>40</v>
-      </c>
-      <c r="H23" s="25">
-        <v>64000</v>
-      </c>
-      <c r="I23" s="24">
-        <v>606502417</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="K23" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L23" s="24" t="s">
-        <v>286</v>
-      </c>
-      <c r="M23" s="24">
-        <v>370</v>
-      </c>
-      <c r="N23" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O23" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P23" s="24" t="s">
-        <v>423</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="T23" s="2"/>
-      <c r="U23" s="24" t="s">
-        <v>314</v>
-      </c>
-      <c r="V23" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>67498</v>
-      </c>
-      <c r="B24" s="2">
-        <v>70022</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="5">
-        <v>32</v>
-      </c>
-      <c r="F24" s="5">
-        <v>38</v>
-      </c>
-      <c r="G24" s="5">
-        <v>50</v>
-      </c>
-      <c r="H24" s="25">
-        <v>75000</v>
-      </c>
-      <c r="I24" s="24">
-        <v>606502419</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="K24" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L24" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="M24" s="24">
-        <v>370</v>
-      </c>
-      <c r="N24" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O24" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P24" s="24" t="s">
-        <v>424</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="R24" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="S24" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="T24" s="2"/>
-      <c r="U24" s="24" t="s">
-        <v>315</v>
-      </c>
-      <c r="V24" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>67404</v>
-      </c>
-      <c r="B25" s="2">
-        <v>70023</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="E25" s="5">
-        <v>36</v>
-      </c>
-      <c r="F25" s="5">
-        <v>46</v>
-      </c>
-      <c r="G25" s="5">
-        <v>50</v>
-      </c>
-      <c r="H25" s="25">
-        <v>90000</v>
-      </c>
-      <c r="I25" s="24">
-        <v>606502421</v>
-      </c>
-      <c r="J25" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="K25" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L25" s="24" t="s">
-        <v>288</v>
-      </c>
-      <c r="M25" s="24">
-        <v>370</v>
-      </c>
-      <c r="N25" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O25" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P25" s="24" t="s">
-        <v>425</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="T25" s="2"/>
-      <c r="U25" s="24" t="s">
-        <v>316</v>
-      </c>
-      <c r="V25" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>67405</v>
-      </c>
-      <c r="B26" s="2">
-        <v>70024</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="10">
-        <v>32</v>
-      </c>
-      <c r="F26" s="10">
-        <v>22</v>
-      </c>
-      <c r="G26" s="10">
-        <v>36</v>
-      </c>
-      <c r="H26" s="25">
-        <v>35000</v>
-      </c>
-      <c r="I26" s="24">
-        <v>606504415</v>
-      </c>
-      <c r="J26" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="K26" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L26" s="24" t="s">
-        <v>289</v>
-      </c>
-      <c r="M26" s="24">
-        <v>370</v>
-      </c>
-      <c r="N26" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O26" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P26" s="24" t="s">
-        <v>426</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="T26" s="2"/>
-      <c r="U26" s="24" t="s">
-        <v>317</v>
-      </c>
-      <c r="V26" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>67406</v>
-      </c>
-      <c r="B27" s="2">
-        <v>70025</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="E27" s="10">
-        <v>34</v>
-      </c>
-      <c r="F27" s="10">
-        <v>24</v>
-      </c>
-      <c r="G27" s="10">
-        <v>40</v>
-      </c>
-      <c r="H27" s="25">
-        <v>64000</v>
-      </c>
-      <c r="I27" s="24">
-        <v>606504418</v>
-      </c>
-      <c r="J27" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="K27" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L27" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="M27" s="24">
-        <v>370</v>
-      </c>
-      <c r="N27" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O27" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P27" s="24" t="s">
-        <v>427</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="T27" s="2"/>
-      <c r="U27" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="V27" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>67407</v>
-      </c>
-      <c r="B28" s="2">
-        <v>70026</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="5">
-        <v>34</v>
-      </c>
-      <c r="F28" s="5">
-        <v>38</v>
-      </c>
-      <c r="G28" s="5">
-        <v>50</v>
-      </c>
-      <c r="H28" s="25">
-        <v>75000</v>
-      </c>
-      <c r="I28" s="24">
-        <v>606504420</v>
-      </c>
-      <c r="J28" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="K28" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L28" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="M28" s="24">
-        <v>370</v>
-      </c>
-      <c r="N28" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O28" s="24">
-        <v>2000179</v>
-      </c>
-      <c r="P28" s="24" t="s">
-        <v>428</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="T28" s="2"/>
-      <c r="U28" s="24" t="s">
-        <v>319</v>
-      </c>
-      <c r="V28" s="24">
-        <v>1</v>
+      <c r="B4" s="24">
+        <v>72441</v>
       </c>
     </row>
   </sheetData>
@@ -3862,7 +1789,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>67393</v>
       </c>
@@ -3947,7 +1874,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>68187</v>
       </c>
@@ -4030,7 +1957,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>67385</v>
       </c>
@@ -4050,7 +1977,7 @@
       <c r="G4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="31" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -4115,7 +2042,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>67386</v>
       </c>
@@ -4135,7 +2062,7 @@
       <c r="G5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="27"/>
+      <c r="H5" s="31"/>
       <c r="I5" s="19" t="s">
         <v>88</v>
       </c>
@@ -4198,7 +2125,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>67387</v>
       </c>
@@ -4218,7 +2145,7 @@
       <c r="G6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="31"/>
       <c r="I6" s="2" t="s">
         <v>89</v>
       </c>
@@ -4281,7 +2208,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>67388</v>
       </c>
@@ -4301,7 +2228,7 @@
       <c r="G7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="27"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="7" t="s">
         <v>90</v>
       </c>
@@ -4360,11 +2287,11 @@
       <c r="AB7" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="AC7" s="26" t="s">
+      <c r="AC7" s="25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>67390</v>
       </c>
@@ -4384,7 +2311,7 @@
       <c r="G8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="27"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="2" t="s">
         <v>91</v>
       </c>
@@ -4447,7 +2374,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>67391</v>
       </c>
@@ -4467,7 +2394,7 @@
       <c r="G9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="27"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="2" t="s">
         <v>92</v>
       </c>
@@ -4530,7 +2457,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>67392</v>
       </c>
@@ -4550,7 +2477,7 @@
       <c r="G10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="27"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="2" t="s">
         <v>93</v>
       </c>
@@ -4613,7 +2540,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>67394</v>
       </c>
@@ -4633,7 +2560,7 @@
       <c r="G11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="27"/>
+      <c r="H11" s="31"/>
       <c r="I11" s="19" t="s">
         <v>201</v>
       </c>
@@ -4641,7 +2568,7 @@
         <v>119</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="L11" s="9">
         <v>15</v>
@@ -4698,7 +2625,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>67395</v>
       </c>
@@ -4718,7 +2645,7 @@
       <c r="G12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="27"/>
+      <c r="H12" s="31"/>
       <c r="I12" s="2" t="s">
         <v>94</v>
       </c>
@@ -4781,7 +2708,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>67396</v>
       </c>
@@ -4801,7 +2728,7 @@
       <c r="G13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="27"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="7" t="s">
         <v>202</v>
       </c>
@@ -4809,7 +2736,7 @@
         <v>119</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="L13" s="9">
         <v>19</v>
@@ -4886,7 +2813,7 @@
       <c r="G14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="32" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -4969,7 +2896,7 @@
       <c r="G15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="29"/>
+      <c r="H15" s="33"/>
       <c r="I15" s="2" t="s">
         <v>96</v>
       </c>
@@ -5026,7 +2953,7 @@
       <c r="AB15" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="AC15" s="26" t="s">
+      <c r="AC15" s="25" t="s">
         <v>78</v>
       </c>
     </row>
@@ -5050,7 +2977,7 @@
       <c r="G16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="29"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="2" t="s">
         <v>97</v>
       </c>
@@ -5131,7 +3058,7 @@
       <c r="G17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="29"/>
+      <c r="H17" s="33"/>
       <c r="I17" s="2" t="s">
         <v>98</v>
       </c>
@@ -5212,7 +3139,7 @@
       <c r="G18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="30" t="s">
+      <c r="H18" s="34" t="s">
         <v>30</v>
       </c>
       <c r="I18" s="2" t="s">
@@ -5293,7 +3220,7 @@
       <c r="G19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="31"/>
+      <c r="H19" s="35"/>
       <c r="I19" s="2" t="s">
         <v>196</v>
       </c>
@@ -5372,7 +3299,7 @@
       <c r="G20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="31"/>
+      <c r="H20" s="35"/>
       <c r="I20" s="2" t="s">
         <v>198</v>
       </c>
@@ -5451,7 +3378,7 @@
       <c r="G21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="32" t="s">
+      <c r="H21" s="36" t="s">
         <v>32</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -5531,7 +3458,7 @@
       <c r="G22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="33"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="2" t="s">
         <v>100</v>
       </c>
@@ -5609,7 +3536,7 @@
       <c r="G23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="33"/>
+      <c r="H23" s="37"/>
       <c r="I23" s="2" t="s">
         <v>101</v>
       </c>
@@ -5687,7 +3614,7 @@
       <c r="G24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="33"/>
+      <c r="H24" s="37"/>
       <c r="I24" s="2" t="s">
         <v>102</v>
       </c>
@@ -5765,7 +3692,7 @@
       <c r="G25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="33"/>
+      <c r="H25" s="37"/>
       <c r="I25" s="2" t="s">
         <v>103</v>
       </c>
@@ -5843,7 +3770,7 @@
       <c r="G26" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H26" s="33"/>
+      <c r="H26" s="37"/>
       <c r="I26" s="2" t="s">
         <v>104</v>
       </c>
@@ -5921,7 +3848,7 @@
       <c r="G27" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H27" s="33"/>
+      <c r="H27" s="37"/>
       <c r="I27" s="2" t="s">
         <v>105</v>
       </c>
@@ -5975,7 +3902,7 @@
       <c r="AB27" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="AC27" s="26" t="s">
+      <c r="AC27" s="25" t="s">
         <v>107</v>
       </c>
     </row>
@@ -5999,7 +3926,7 @@
       <c r="G28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H28" s="33"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="2" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
new feat verifying id, big refactoring in modules and structure
</commit_message>
<xml_diff>
--- a/planilhapadrão/Hercules Cobaia.xlsx
+++ b/planilhapadrão/Hercules Cobaia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Python\automatizar_planilha_vtex\planilhapadrão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3494C9C-828B-4823-B764-44880B80D6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA251679-318E-4D76-950A-A4203E0ED32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A220D98B-D511-4261-A1DE-F69C6B222EA8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="277">
   <si>
     <t>_SkuEan</t>
   </si>
@@ -910,6 +910,9 @@
   </si>
   <si>
     <t>Vídeo do produto</t>
+  </si>
+  <si>
+    <t>motor-monofasico-hercules-ip-21-4p-3-</t>
   </si>
 </sst>
 </file>
@@ -1514,10 +1517,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6BD081A-DEC6-48D2-AA98-0A6163BE7B71}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1671,13 +1674,67 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <v>67390</v>
+      </c>
       <c r="B3" s="30">
-        <v>72447</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24">
-        <v>72441</v>
+        <v>72451</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="28">
+        <v>26</v>
+      </c>
+      <c r="F3" s="28">
+        <v>24</v>
+      </c>
+      <c r="G3" s="28">
+        <v>43</v>
+      </c>
+      <c r="H3" s="29">
+        <v>22000</v>
+      </c>
+      <c r="I3" s="27">
+        <v>605012134</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="M3" s="27">
+        <v>370</v>
+      </c>
+      <c r="N3" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="O3" s="27">
+        <v>2000179</v>
+      </c>
+      <c r="P3" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q3" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="S3" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="T3" s="26"/>
+      <c r="U3" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="V3" s="27">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solving bug in id's verification
</commit_message>
<xml_diff>
--- a/planilhapadrão/Hercules Cobaia.xlsx
+++ b/planilhapadrão/Hercules Cobaia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Python\automatizar_planilha_vtex\planilhapadrão\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA251679-318E-4D76-950A-A4203E0ED32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD509C0E-53B3-4A57-934B-606D7C7E3D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A220D98B-D511-4261-A1DE-F69C6B222EA8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A220D98B-D511-4261-A1DE-F69C6B222EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixa" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="289">
   <si>
     <t>_SkuEan</t>
   </si>
@@ -913,6 +913,42 @@
   </si>
   <si>
     <t>motor-monofasico-hercules-ip-21-4p-3-</t>
+  </si>
+  <si>
+    <t>70001DESC</t>
+  </si>
+  <si>
+    <t>70002DESC</t>
+  </si>
+  <si>
+    <t>70002FOR</t>
+  </si>
+  <si>
+    <t>70001FOR</t>
+  </si>
+  <si>
+    <t>70002TEC</t>
+  </si>
+  <si>
+    <t>70001TEC</t>
+  </si>
+  <si>
+    <t>70003TEC</t>
+  </si>
+  <si>
+    <t>70003FOR</t>
+  </si>
+  <si>
+    <t>70003DESC</t>
+  </si>
+  <si>
+    <t>70003Hércules</t>
+  </si>
+  <si>
+    <t>70001Hércules</t>
+  </si>
+  <si>
+    <t>70002Hércules</t>
   </si>
 </sst>
 </file>
@@ -1517,10 +1553,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6BD081A-DEC6-48D2-AA98-0A6163BE7B71}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1614,7 +1650,7 @@
         <v>67393</v>
       </c>
       <c r="B2" s="30">
-        <v>72450</v>
+        <v>72481</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>77</v>
@@ -1678,7 +1714,7 @@
         <v>67390</v>
       </c>
       <c r="B3" s="30">
-        <v>72451</v>
+        <v>72480</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>77</v>
@@ -1718,22 +1754,150 @@
         <v>2000179</v>
       </c>
       <c r="P3" s="27" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="Q3" s="26" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="R3" s="26" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="S3" s="26" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="T3" s="26"/>
       <c r="U3" s="27" t="s">
         <v>276</v>
       </c>
       <c r="V3" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>67391</v>
+      </c>
+      <c r="B4" s="30">
+        <v>72479</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28">
+        <v>26</v>
+      </c>
+      <c r="F4" s="28">
+        <v>24</v>
+      </c>
+      <c r="G4" s="28">
+        <v>43</v>
+      </c>
+      <c r="H4" s="29">
+        <v>22000</v>
+      </c>
+      <c r="I4" s="27">
+        <v>605012134</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="M4" s="27">
+        <v>370</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="O4" s="27">
+        <v>2000179</v>
+      </c>
+      <c r="P4" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q4" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="R4" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="S4" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="T4" s="26"/>
+      <c r="U4" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="V4" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>67392</v>
+      </c>
+      <c r="B5" s="24">
+        <v>72478</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28">
+        <v>26</v>
+      </c>
+      <c r="F5" s="28">
+        <v>24</v>
+      </c>
+      <c r="G5" s="28">
+        <v>43</v>
+      </c>
+      <c r="H5" s="29">
+        <v>22000</v>
+      </c>
+      <c r="I5" s="27">
+        <v>605012134</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="M5" s="27">
+        <v>370</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="O5" s="27">
+        <v>2000179</v>
+      </c>
+      <c r="P5" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="S5" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="T5" s="26"/>
+      <c r="U5" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="V5" s="27">
         <v>2</v>
       </c>
     </row>

</xml_diff>